<commit_message>
Modificacion de tabla zona
</commit_message>
<xml_diff>
--- a/archivos2 - copia/2019-12-DICIEMBRE/2019-12-DICIEMBRE/comisiones/AVANCEVENDEDOR.xlsx
+++ b/archivos2 - copia/2019-12-DICIEMBRE/2019-12-DICIEMBRE/comisiones/AVANCEVENDEDOR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stipro\comisiones2\archivos2 - copia\2019-12-DICIEMBRE\2019-12-DICIEMBRE\comisiones\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D21205A-7E2E-4338-908C-1D9B18D46628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F23B75-8A3D-4145-84ED-50C6F5275FDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1752" yWindow="1896" windowWidth="11460" windowHeight="10464" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AVANCEVENDEDOR" sheetId="1" r:id="rId1"/>
@@ -1289,7 +1289,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1304,12 +1304,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1347,7 +1341,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="265">
+  <cellXfs count="262">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1605,14 +1599,11 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="248" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="248" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="14" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="248" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="14" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="248" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="14" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="248" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1941,7 +1932,7 @@
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -2001,44 +1992,44 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="261" customFormat="1">
+    <row r="2" spans="1:13" s="258" customFormat="1">
       <c r="A2" s="169" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="169" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="260">
+      <c r="C2" s="257">
         <v>167709.12</v>
       </c>
-      <c r="D2" s="260">
+      <c r="D2" s="257">
         <v>2137.86</v>
       </c>
-      <c r="E2" s="260">
+      <c r="E2" s="257">
         <v>165571.26</v>
       </c>
-      <c r="F2" s="260">
+      <c r="F2" s="257">
         <v>171400.75</v>
       </c>
-      <c r="G2" s="260">
+      <c r="G2" s="257">
         <v>96.6</v>
       </c>
-      <c r="H2" s="260">
+      <c r="H2" s="257">
         <v>94</v>
       </c>
-      <c r="I2" s="260">
+      <c r="I2" s="257">
         <v>83</v>
       </c>
-      <c r="J2" s="260">
+      <c r="J2" s="257">
         <v>208511.72</v>
       </c>
-      <c r="K2" s="260">
+      <c r="K2" s="257">
         <v>289721.56</v>
       </c>
-      <c r="L2" s="260">
+      <c r="L2" s="257">
         <v>4.6500000000000004</v>
       </c>
-      <c r="M2" s="260">
+      <c r="M2" s="257">
         <v>13477.84</v>
       </c>
     </row>
@@ -2206,85 +2197,85 @@
         <v>33178.550000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:13" s="259" customFormat="1">
-      <c r="A7" s="257" t="s">
+    <row r="7" spans="1:13" s="261" customFormat="1">
+      <c r="A7" s="259" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="257" t="s">
+      <c r="B7" s="259" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="258">
+      <c r="C7" s="260">
         <v>173583.6</v>
       </c>
-      <c r="D7" s="258">
+      <c r="D7" s="260">
         <v>6318.89</v>
       </c>
-      <c r="E7" s="258">
+      <c r="E7" s="260">
         <v>167264.71</v>
       </c>
-      <c r="F7" s="258">
+      <c r="F7" s="260">
         <v>350211.82</v>
       </c>
-      <c r="G7" s="258">
+      <c r="G7" s="260">
         <v>47.76</v>
       </c>
-      <c r="H7" s="258">
+      <c r="H7" s="260">
         <v>15</v>
       </c>
-      <c r="I7" s="258">
+      <c r="I7" s="260">
         <v>10</v>
       </c>
-      <c r="J7" s="258">
+      <c r="J7" s="260">
         <v>451561.19</v>
       </c>
-      <c r="K7" s="258">
+      <c r="K7" s="260">
         <v>692118.64</v>
       </c>
-      <c r="L7" s="258">
+      <c r="L7" s="260">
         <v>1.76</v>
       </c>
-      <c r="M7" s="258">
+      <c r="M7" s="260">
         <v>12189.77</v>
       </c>
     </row>
-    <row r="8" spans="1:13" s="261" customFormat="1">
+    <row r="8" spans="1:13" s="258" customFormat="1">
       <c r="A8" s="169" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="169" t="s">
         <v>77</v>
       </c>
-      <c r="C8" s="260">
+      <c r="C8" s="257">
         <v>282029.05</v>
       </c>
-      <c r="D8" s="260">
+      <c r="D8" s="257">
         <v>5570</v>
       </c>
-      <c r="E8" s="260">
+      <c r="E8" s="257">
         <v>276459.05</v>
       </c>
-      <c r="F8" s="260">
+      <c r="F8" s="257">
         <v>276233.59000000003</v>
       </c>
-      <c r="G8" s="260">
+      <c r="G8" s="257">
         <v>100.08</v>
       </c>
-      <c r="H8" s="260">
+      <c r="H8" s="257">
         <v>80</v>
       </c>
-      <c r="I8" s="260">
+      <c r="I8" s="257">
         <v>45</v>
       </c>
-      <c r="J8" s="260">
+      <c r="J8" s="257">
         <v>327057.65000000002</v>
       </c>
-      <c r="K8" s="260">
+      <c r="K8" s="257">
         <v>691894.11</v>
       </c>
-      <c r="L8" s="260">
+      <c r="L8" s="257">
         <v>4.53</v>
       </c>
-      <c r="M8" s="260">
+      <c r="M8" s="257">
         <v>31381.71</v>
       </c>
     </row>
@@ -2657,85 +2648,85 @@
         <v>1093819.8700000001</v>
       </c>
     </row>
-    <row r="18" spans="1:13" s="259" customFormat="1">
-      <c r="A18" s="257" t="s">
+    <row r="18" spans="1:13" s="258" customFormat="1">
+      <c r="A18" s="169" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="257" t="s">
+      <c r="B18" s="169" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="258">
-        <v>0</v>
-      </c>
-      <c r="D18" s="258">
-        <v>0</v>
-      </c>
-      <c r="E18" s="258">
-        <v>0</v>
-      </c>
-      <c r="F18" s="258">
-        <v>0</v>
-      </c>
-      <c r="G18" s="258">
-        <v>0</v>
-      </c>
-      <c r="H18" s="258">
+      <c r="C18" s="257">
+        <v>0</v>
+      </c>
+      <c r="D18" s="257">
+        <v>0</v>
+      </c>
+      <c r="E18" s="257">
+        <v>0</v>
+      </c>
+      <c r="F18" s="257">
+        <v>0</v>
+      </c>
+      <c r="G18" s="257">
+        <v>0</v>
+      </c>
+      <c r="H18" s="257">
         <v>2</v>
       </c>
-      <c r="I18" s="258">
-        <v>0</v>
-      </c>
-      <c r="J18" s="258">
-        <v>0</v>
-      </c>
-      <c r="K18" s="258">
-        <v>0</v>
-      </c>
-      <c r="L18" s="258">
-        <v>0</v>
-      </c>
-      <c r="M18" s="258">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" s="264" customFormat="1">
-      <c r="A19" s="262" t="s">
+      <c r="I18" s="257">
+        <v>0</v>
+      </c>
+      <c r="J18" s="257">
+        <v>0</v>
+      </c>
+      <c r="K18" s="257">
+        <v>0</v>
+      </c>
+      <c r="L18" s="257">
+        <v>0</v>
+      </c>
+      <c r="M18" s="257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="258" customFormat="1">
+      <c r="A19" s="169" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="262" t="s">
+      <c r="B19" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="263">
+      <c r="C19" s="257">
         <v>74586.100000000006</v>
       </c>
-      <c r="D19" s="263">
+      <c r="D19" s="257">
         <v>1282.29</v>
       </c>
-      <c r="E19" s="263">
+      <c r="E19" s="257">
         <v>73303.81</v>
       </c>
-      <c r="F19" s="263">
+      <c r="F19" s="257">
         <v>83100</v>
       </c>
-      <c r="G19" s="263">
+      <c r="G19" s="257">
         <v>88.21</v>
       </c>
-      <c r="H19" s="263">
+      <c r="H19" s="257">
         <v>204</v>
       </c>
-      <c r="I19" s="263">
+      <c r="I19" s="257">
         <v>117</v>
       </c>
-      <c r="J19" s="263">
+      <c r="J19" s="257">
         <v>100616.91</v>
       </c>
-      <c r="K19" s="263">
+      <c r="K19" s="257">
         <v>18460.400000000001</v>
       </c>
-      <c r="L19" s="263">
+      <c r="L19" s="257">
         <v>1.64</v>
       </c>
-      <c r="M19" s="263">
+      <c r="M19" s="257">
         <v>303.12</v>
       </c>
     </row>
@@ -2821,85 +2812,85 @@
         <v>17675.810000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:13" s="256" customFormat="1">
-      <c r="A22" s="254" t="s">
+    <row r="22" spans="1:13" s="258" customFormat="1">
+      <c r="A22" s="169" t="s">
         <v>51</v>
       </c>
-      <c r="B22" s="254" t="s">
+      <c r="B22" s="169" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="255">
+      <c r="C22" s="257">
         <v>617.25</v>
       </c>
-      <c r="D22" s="255">
-        <v>0</v>
-      </c>
-      <c r="E22" s="255">
+      <c r="D22" s="257">
+        <v>0</v>
+      </c>
+      <c r="E22" s="257">
         <v>617.25</v>
       </c>
-      <c r="F22" s="255">
-        <v>0</v>
-      </c>
-      <c r="G22" s="255">
-        <v>0</v>
-      </c>
-      <c r="H22" s="255">
+      <c r="F22" s="257">
+        <v>0</v>
+      </c>
+      <c r="G22" s="257">
+        <v>0</v>
+      </c>
+      <c r="H22" s="257">
         <v>136</v>
       </c>
-      <c r="I22" s="255">
+      <c r="I22" s="257">
         <v>2</v>
       </c>
-      <c r="J22" s="255">
+      <c r="J22" s="257">
         <v>728.35</v>
       </c>
-      <c r="K22" s="255">
-        <v>0</v>
-      </c>
-      <c r="L22" s="255">
-        <v>0</v>
-      </c>
-      <c r="M22" s="255">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" s="261" customFormat="1">
+      <c r="K22" s="257">
+        <v>0</v>
+      </c>
+      <c r="L22" s="257">
+        <v>0</v>
+      </c>
+      <c r="M22" s="257">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="258" customFormat="1">
       <c r="A23" s="169" t="s">
         <v>53</v>
       </c>
       <c r="B23" s="169" t="s">
         <v>54</v>
       </c>
-      <c r="C23" s="260">
-        <v>0</v>
-      </c>
-      <c r="D23" s="260">
-        <v>0</v>
-      </c>
-      <c r="E23" s="260">
-        <v>0</v>
-      </c>
-      <c r="F23" s="260">
-        <v>0</v>
-      </c>
-      <c r="G23" s="260">
-        <v>0</v>
-      </c>
-      <c r="H23" s="260">
+      <c r="C23" s="257">
+        <v>0</v>
+      </c>
+      <c r="D23" s="257">
+        <v>0</v>
+      </c>
+      <c r="E23" s="257">
+        <v>0</v>
+      </c>
+      <c r="F23" s="257">
+        <v>0</v>
+      </c>
+      <c r="G23" s="257">
+        <v>0</v>
+      </c>
+      <c r="H23" s="257">
         <v>85</v>
       </c>
-      <c r="I23" s="260">
-        <v>0</v>
-      </c>
-      <c r="J23" s="260">
+      <c r="I23" s="257">
+        <v>0</v>
+      </c>
+      <c r="J23" s="257">
         <v>2000</v>
       </c>
-      <c r="K23" s="260">
+      <c r="K23" s="257">
         <v>17115.84</v>
       </c>
-      <c r="L23" s="260">
+      <c r="L23" s="257">
         <v>100</v>
       </c>
-      <c r="M23" s="260">
+      <c r="M23" s="257">
         <v>17115.84</v>
       </c>
     </row>
@@ -2985,44 +2976,44 @@
         <v>56.03</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="261" customFormat="1">
+    <row r="26" spans="1:13" s="258" customFormat="1">
       <c r="A26" s="169" t="s">
         <v>59</v>
       </c>
       <c r="B26" s="169" t="s">
         <v>60</v>
       </c>
-      <c r="C26" s="260">
+      <c r="C26" s="257">
         <v>125002.56</v>
       </c>
-      <c r="D26" s="260">
+      <c r="D26" s="257">
         <v>2527.87</v>
       </c>
-      <c r="E26" s="260">
+      <c r="E26" s="257">
         <v>122474.69</v>
       </c>
-      <c r="F26" s="260">
+      <c r="F26" s="257">
         <v>143512.35</v>
       </c>
-      <c r="G26" s="260">
+      <c r="G26" s="257">
         <v>85.34</v>
       </c>
-      <c r="H26" s="260">
+      <c r="H26" s="257">
         <v>79</v>
       </c>
-      <c r="I26" s="260">
+      <c r="I26" s="257">
         <v>29</v>
       </c>
-      <c r="J26" s="260">
+      <c r="J26" s="257">
         <v>118204.35</v>
       </c>
-      <c r="K26" s="260">
+      <c r="K26" s="257">
         <v>359891.08</v>
       </c>
-      <c r="L26" s="260">
+      <c r="L26" s="257">
         <v>26.14</v>
       </c>
-      <c r="M26" s="260">
+      <c r="M26" s="257">
         <v>94070.74</v>
       </c>
     </row>
@@ -3067,44 +3058,44 @@
         <v>79929.37</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="264" customFormat="1">
-      <c r="A28" s="262" t="s">
+    <row r="28" spans="1:13" s="258" customFormat="1">
+      <c r="A28" s="169" t="s">
         <v>63</v>
       </c>
-      <c r="B28" s="262" t="s">
+      <c r="B28" s="169" t="s">
         <v>64</v>
       </c>
-      <c r="C28" s="263">
+      <c r="C28" s="257">
         <v>145280.60999999999</v>
       </c>
-      <c r="D28" s="263">
+      <c r="D28" s="257">
         <v>2513.4499999999998</v>
       </c>
-      <c r="E28" s="263">
+      <c r="E28" s="257">
         <v>142767.16</v>
       </c>
-      <c r="F28" s="263">
+      <c r="F28" s="257">
         <v>228451.88</v>
       </c>
-      <c r="G28" s="263">
+      <c r="G28" s="257">
         <v>62.49</v>
       </c>
-      <c r="H28" s="263">
+      <c r="H28" s="257">
         <v>60</v>
       </c>
-      <c r="I28" s="263">
+      <c r="I28" s="257">
         <v>35</v>
       </c>
-      <c r="J28" s="263">
+      <c r="J28" s="257">
         <v>266571.09999999998</v>
       </c>
-      <c r="K28" s="263">
+      <c r="K28" s="257">
         <v>467883.11</v>
       </c>
-      <c r="L28" s="263">
+      <c r="L28" s="257">
         <v>11.61</v>
       </c>
-      <c r="M28" s="263">
+      <c r="M28" s="257">
         <v>54352.26</v>
       </c>
     </row>

</xml_diff>